<commit_message>
-Modified object-analysis.xslx to show new changes - Added uml class diagrams for JSONLoader, NewsTicker and NewsTickerItem - Added RequireJS to the project for AMD management - Created JSONLoader, NewsTicker and NewsTickerItem intefaces - Added Handlebars and created pre-compiled Handlebars template for   NewsTicker
</commit_message>
<xml_diff>
--- a/report/object-analysis.xlsx
+++ b/report/object-analysis.xlsx
@@ -7,16 +7,14 @@
     <workbookView xWindow="120" yWindow="120" windowWidth="19020" windowHeight="8070"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="object-analysis" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>PaginationDevice</t>
   </si>
@@ -99,13 +97,31 @@
     <t>JSONDidLoad</t>
   </si>
   <si>
-    <t>NewsTickerItemSport</t>
-  </si>
-  <si>
-    <t>1, 2</t>
-  </si>
-  <si>
     <t>User</t>
+  </si>
+  <si>
+    <t>Accountable for behaviours</t>
+  </si>
+  <si>
+    <t>Load JSON from external source</t>
+  </si>
+  <si>
+    <t>Add news item to ticker</t>
+  </si>
+  <si>
+    <t>Alert system once JSON is loaded (JSONDidLoad)</t>
+  </si>
+  <si>
+    <t>Alert system when a paginated button is clicked (NewsTickerBeginNavigation)</t>
+  </si>
+  <si>
+    <t>Build pagination device from news items (conforming to GEL)</t>
+  </si>
+  <si>
+    <t>Contain the details of a news story</t>
+  </si>
+  <si>
+    <t>2,</t>
   </si>
 </sst>
 </file>
@@ -267,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -281,6 +297,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,25 +599,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -608,7 +626,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -616,7 +634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -624,157 +642,211 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="C7" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="11"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="B10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="C15" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="11"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="B16" s="11"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="11"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="11"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="B18" s="11"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="11"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="B26" s="11"/>
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="11"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="11"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="B28" s="11"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="11"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="B32" s="11"/>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="13"/>
     </row>
   </sheetData>
   <sortState ref="A7:B15">
@@ -783,28 +855,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>